<commit_message>
Dynamic values for email implemented
</commit_message>
<xml_diff>
--- a/Data/ConfigFile.xlsx
+++ b/Data/ConfigFile.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dee\Documents\UiPath\Assignment2-NotGreat\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DE42C9-3CB5-49C8-AAD8-DBB259FA4B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817F11F3-B98B-4DE4-BD48-3B0D67A8DA51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5205" yWindow="1860" windowWidth="21600" windowHeight="7575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
+    <sheet name="Email" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -66,9 +67,6 @@
     <t>carModel2</t>
   </si>
   <si>
-    <t>Volkswagen</t>
-  </si>
-  <si>
     <t>up!</t>
   </si>
   <si>
@@ -78,17 +76,62 @@
     <t>ForTwo</t>
   </si>
   <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t>Germania</t>
+    <t>name</t>
+  </si>
+  <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t>diana.gradinaru.sincai@gmail.com</t>
+  </si>
+  <si>
+    <t>Make for the first selected car</t>
+  </si>
+  <si>
+    <t>Model for the first selected car</t>
+  </si>
+  <si>
+    <t>Make for the second selected car</t>
+  </si>
+  <si>
+    <t>Model for the second selected car</t>
+  </si>
+  <si>
+    <t>Email address</t>
+  </si>
+  <si>
+    <t>Name of the person</t>
+  </si>
+  <si>
+    <t>Body of the email</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Delia</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>Assignment number 2 done</t>
+  </si>
+  <si>
+    <t>Salut,
+Atasez excelul aferent punctului 2 din assignment.
+Multumesc,
+Diana Gradinaru</t>
+  </si>
+  <si>
+    <t>qwsdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +149,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -128,14 +179,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -414,17 +471,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
     <col min="2" max="2" width="53.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -454,7 +511,10 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -462,7 +522,10 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -470,7 +533,10 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -478,15 +544,10 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -497,4 +558,78 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74FD7139-8690-4DCE-B7CC-B31A9223EBAE}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="74.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{2ACD65EA-540C-4EDF-A5A3-21CC908E1E35}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>